<commit_message>
login signout forgot password
</commit_message>
<xml_diff>
--- a/src/main/resources/BuffalocartTestData.xlsx
+++ b/src/main/resources/BuffalocartTestData.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manua\eclipse-workspace\buffalocart\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B265FA4-FB73-4C9A-A149-91BC39671524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF889B6B-85E7-4731-949B-1FDD04DA18BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="UserEmail" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>username</t>
   </si>
@@ -37,16 +38,30 @@
   </si>
   <si>
     <t>user</t>
+  </si>
+  <si>
+    <t>emailid</t>
+  </si>
+  <si>
+    <t>manuav2003@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -69,13 +84,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -354,10 +372,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -386,7 +404,41 @@
         <v>3</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5223BDA8-FE77-4512-A101-A3B59B0F948F}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="26.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{60DB9599-93E1-4930-8ED0-D5A467FD895E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>